<commit_message>
update specialty email test file
</commit_message>
<xml_diff>
--- a/test_files/Specialty Emailed Version.xlsx
+++ b/test_files/Specialty Emailed Version.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Table" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$U$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Table!$A$1:$U$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -499,7 +499,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -511,7 +511,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>